<commit_message>
Edit/create project page: search removed, daterangepicker split into 2.
</commit_message>
<xml_diff>
--- a/src/main/AllyisApps/Resources/Files/CustomerProjectImportTemplate.xlsx
+++ b/src/main/AllyisApps/Resources/Files/CustomerProjectImportTemplate.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="AboutImporting" sheetId="3" r:id="rId1"/>
+    <sheet name="About Importing" sheetId="3" r:id="rId1"/>
     <sheet name="Customers" sheetId="2" r:id="rId2"/>
     <sheet name="Projects" sheetId="1" r:id="rId3"/>
   </sheets>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
   <si>
     <t>Project Name</t>
   </si>
@@ -32,12 +32,6 @@
     <t>Customer Id</t>
   </si>
   <si>
-    <t>&lt;-(Required)</t>
-  </si>
-  <si>
-    <t>(Optional)-&gt;</t>
-  </si>
-  <si>
     <t>Project Type</t>
   </si>
   <si>
@@ -83,15 +77,9 @@
     <t>Fixed</t>
   </si>
   <si>
-    <t>(Required:)</t>
-  </si>
-  <si>
     <t>Customer Name</t>
   </si>
   <si>
-    <t>(Optional:)</t>
-  </si>
-  <si>
     <t>Customer Street Address</t>
   </si>
   <si>
@@ -167,15 +155,12 @@
     <t>Importing Customers and Projects</t>
   </si>
   <si>
-    <t xml:space="preserve">     To import customers and/or projects in bulk from a spreadsheet, all you need is to have your data organized under the correct column headers. AllyisApps will recognize the column header names and import the items on each row. See the other worksheets in this workbook for examples.
-     For customers, the required columns are Customer Name and Customer Id (note the lowercase d). You must have both to import a customer. Optionally, you can also include Customer Street Address, Customer City, Customer Country, Customer State, Customer Postal Code, Customer Email, Customer Phone Number, Customer Fax Number, and/or Customer EIN.
-     For projects, you must have the columns Project Name and Project Id, as well as either Customer Name or Customer Id. Projects must be linked to a customer. It is not necessary to have all three pieces of required information on the same worksheet, as long as some worksheet exists in the workbook that completes each project. For example, you could have a worksheet with Project Name and Project Id, and another with Project Name and Customer Id. The import function will see this and try to find the missing information by linking together the two using the common column of Project Name. As with customers, you can also include optional information for projects. The optional columns are Project Type, Project Start Date and Project End Date.
-     There is no required order for the worksheets. You can have customers first, or projects first, or multiple worksheets with information for each in various combinations. As long as each customer or project you wish to import has all the required information present and linkable somewhere in the workbook, they will be imported. If not all the required information is there, or no common columns can be used to link it together, you will see a corresponding error notification at the end of the import.
-     Any unrecognized column headers will simply be ignored, as will blank rows. For example, this "AboutImporting" worksheet will have no effect on an import because it contains no relevant column headers.
-     You do not have to import customers/projects separately from users or time entries. All can be imported at once from the same workbook, and all import links on AllyisApps can import any type of information, regardless of where on the site you get to it from. See the Template examples from the Add User page and Time Entry Index page for information on importing users and time entries.</t>
-  </si>
-  <si>
     <t>Washington</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     This workbook demonstrates how to import customers and projects in bulk. Required columns have bold column headers in this example (you don't need to use bold for importing), and optional column headers are not bold. It is important that you spell the columns headers exactly as you see them here, but it does not matter what order the columns are in or if there are additional columns with other headers (they will be ignored). You may have empty cells in any of the non-required columns, but leaving out any of the information in the (bold) required columns will result in an error and a failure to import that customer or project.
+     The next sheet ("Customers") shows what you need to import customers, and the following sheet ("Projects) shows what you need for projects. In this example, "Customer Id" is used to identify which customer a project should fall under, but you could alternatively use "Customer Name" the same way. If you do not provide the optional information for "Project Type", "Project Start Date", or "Project End Date", the imported project will have default values ("Hourly", today's date, and 6 months from now, respectively).
+     You can import both customers and projects at once using different sheets in the same workbook, as shown here. Or, you can import them in separate files. In that case, be sure to import customers first.</t>
   </si>
 </sst>
 </file>
@@ -1035,8 +1020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,13 +1031,13 @@
   <sheetData>
     <row r="1" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:1" ht="384.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="200.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1062,145 +1047,136 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="1.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2">
+        <v>98765</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s">
         <v>32</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J2">
-        <v>98765</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="L2" t="s">
-        <v>38</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="F3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3">
+        <v>99999</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="N2" t="s">
+      <c r="I3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="J3" t="s">
         <v>41</v>
       </c>
-      <c r="G3" t="s">
+      <c r="K3" t="s">
         <v>42</v>
-      </c>
-      <c r="H3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J3">
-        <v>99999</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="L3" t="s">
-        <v>44</v>
-      </c>
-      <c r="M3" t="s">
-        <v>45</v>
-      </c>
-      <c r="N3" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1"/>
-    <hyperlink ref="K3" r:id="rId2"/>
+    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="H3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1208,10 +1184,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1219,16 +1195,12 @@
     <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="1.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="1.7109375" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1238,90 +1210,84 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="E1" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1">
+        <v>42614</v>
+      </c>
+      <c r="F2" s="1">
+        <v>42979</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="1">
-        <v>42614</v>
-      </c>
-      <c r="J2" s="1">
-        <v>42979</v>
+      <c r="E3" s="1">
+        <v>42658</v>
+      </c>
+      <c r="F3" s="1">
+        <v>42840</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="1">
-        <v>42658</v>
-      </c>
-      <c r="J3" s="1">
-        <v>42840</v>
+      <c r="C4" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="D5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="1">
+      <c r="E5" s="1">
         <v>42719</v>
       </c>
-      <c r="J5" s="1">
+      <c r="F5" s="1">
         <v>43266</v>
       </c>
     </row>

</xml_diff>